<commit_message>
Made the test pass
</commit_message>
<xml_diff>
--- a/resources/excel/abs_import_sheet(valid_1).xlsx
+++ b/resources/excel/abs_import_sheet(valid_1).xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Documents/Werk/abs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Documents/work/eclipse-workspace/abs-excel-converter/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Import-ID</t>
   </si>
@@ -53,21 +53,6 @@
     <t>Status x</t>
   </si>
   <si>
-    <t>weg</t>
-  </si>
-  <si>
-    <t>markering</t>
-  </si>
-  <si>
-    <t>lijn links</t>
-  </si>
-  <si>
-    <t>bebording</t>
-  </si>
-  <si>
-    <t>Obxxxyyzz</t>
-  </si>
-  <si>
     <t>As-designed</t>
   </si>
   <si>
@@ -78,19 +63,50 @@
   </si>
   <si>
     <t>RC 237</t>
+  </si>
+  <si>
+    <t>lantaarnpaal</t>
+  </si>
+  <si>
+    <t>OB00833</t>
+  </si>
+  <si>
+    <t>lamp</t>
+  </si>
+  <si>
+    <t>OB00836</t>
+  </si>
+  <si>
+    <t>steun</t>
+  </si>
+  <si>
+    <t>c123f4k31d</t>
+  </si>
+  <si>
+    <t>OB00454</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF777777"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Monaco"/>
     </font>
   </fonts>
   <fills count="2">
@@ -113,8 +129,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,12 +412,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="184" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScale="185" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" customWidth="1"/>
     <col min="4" max="4" width="18.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
@@ -436,87 +456,67 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>821</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>821</v>
+      </c>
+      <c r="G5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="H5" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="G6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -540,10 +540,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G12" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="H12" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>